<commit_message>
MPI-MiS and Kentucky University-Wide materials
</commit_message>
<xml_diff>
--- a/Postdocs19.xlsx
+++ b/Postdocs19.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DJBruce/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DJBruce/Application-Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F912B65A-1D8F-A047-9954-FEB4A53AC25B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038F8069-594C-F544-AC84-8D5662198771}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" xr2:uid="{FC4BAEE4-913F-A74A-BB8A-E591CDEA97CC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" activeTab="1" xr2:uid="{FC4BAEE4-913F-A74A-BB8A-E591CDEA97CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Letters" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="168">
   <si>
     <t xml:space="preserve">Arizona State University </t>
   </si>
@@ -430,6 +431,111 @@
   </si>
   <si>
     <t>https://apply.interfolio.com/67247</t>
+  </si>
+  <si>
+    <t>University of Edinburgh</t>
+  </si>
+  <si>
+    <t>713-WRF</t>
+  </si>
+  <si>
+    <t>https://www.vacancies.ed.ac.uk/pls/corehrrecruit/erq_jobspec_version_4.jobspec?p_id=050154.</t>
+  </si>
+  <si>
+    <t>a file entitled YYY.pdf where YYY must equal one of ACM, AP, OORS, SS or MSE indicating to which theme (see above) the research is most closely related. This one page file should be anonymous, so not have reference to your name or your co-authors (references can be numbered, referring to your publication list). It must include a five word descriptor of your research area; indicate the number of years since you completed your PhD (excluding career breaks); and give a concise summary of your existing research achievements.</t>
+  </si>
+  <si>
+    <t>University of Oxford</t>
+  </si>
+  <si>
+    <t>473-TITCHMARSH2020</t>
+  </si>
+  <si>
+    <t> https://www.recruit.ox.ac.uk/pls/hrisliverecruit/erq_jobspec_version_4.jobspec?p_id=143481</t>
+  </si>
+  <si>
+    <t>You will be required to upload a supporting letter setting out how you meet the selection criteria, a curriculum vitae including full list of publications with top three papers starred</t>
+  </si>
+  <si>
+    <t>Syracuse University</t>
+  </si>
+  <si>
+    <t>SU-RPD</t>
+  </si>
+  <si>
+    <t>Step 1. Candidates must submit an online application with a CV on this website, http://www.sujobopps.com/postings/82133.</t>
+  </si>
+  <si>
+    <t>Cambridge University</t>
+  </si>
+  <si>
+    <t>CambUK-HSRF</t>
+  </si>
+  <si>
+    <t>http://www.dpmms.cam.ac.uk/job/23670</t>
+  </si>
+  <si>
+    <t>Yes, 2 pages</t>
+  </si>
+  <si>
+    <t>Yes, best 3</t>
+  </si>
+  <si>
+    <t>A one page summary of your proposed project, and project description.</t>
+  </si>
+  <si>
+    <t>UofT-PDF</t>
+  </si>
+  <si>
+    <t>Teaching Dossier (include teaching evaluations) </t>
+  </si>
+  <si>
+    <t>Daniel Erman</t>
+  </si>
+  <si>
+    <t>Christine Berkesch</t>
+  </si>
+  <si>
+    <t>Kiran Kedlaya</t>
+  </si>
+  <si>
+    <t>David Eisenbud</t>
+  </si>
+  <si>
+    <t>Shirin Malekpour</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Upload 9/30/19</t>
+  </si>
+  <si>
+    <t>Upload 10/14/19</t>
+  </si>
+  <si>
+    <t>Upload 9/24/19</t>
+  </si>
+  <si>
+    <t>Upload 10/22/19</t>
+  </si>
+  <si>
+    <t>Upload 10/21/19</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Requested 10/21/19</t>
+  </si>
+  <si>
+    <t>Re-Request 10/21/19</t>
+  </si>
+  <si>
+    <t>Request Need</t>
+  </si>
+  <si>
+    <t>Request Needed</t>
   </si>
 </sst>
 </file>
@@ -460,7 +566,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -473,8 +579,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF5D6C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -605,12 +729,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -686,6 +819,52 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -694,6 +873,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5D6C"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1002,11 +1186,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C862073-6331-234F-B2D0-82C360D0D85F}">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1361,56 +1545,58 @@
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="10">
-        <v>43773</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="7">
+      <c r="A9" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="12">
+        <v>43770</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="11">
         <v>3</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="11">
         <v>1</v>
       </c>
-      <c r="M9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="7"/>
+      <c r="M9" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="10">
-        <v>43784</v>
+        <v>43773</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>2</v>
@@ -1428,16 +1614,16 @@
         <v>20</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>27</v>
+      <c r="K10" s="7">
+        <v>3</v>
+      </c>
+      <c r="L10" s="7">
+        <v>1</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>23</v>
@@ -1446,10 +1632,10 @@
     </row>
     <row r="11" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C11" s="10">
         <v>43784</v>
@@ -1475,67 +1661,65 @@
       <c r="J11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="10">
+        <v>43784</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="7">
         <v>3</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L12" s="7">
         <v>1</v>
       </c>
-      <c r="M11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N11" s="7"/>
-    </row>
-    <row r="12" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C12" s="12">
-        <v>43784</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="11">
-        <v>3</v>
-      </c>
-      <c r="L12" s="11">
-        <v>1</v>
-      </c>
       <c r="M12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N12" s="19" t="s">
-        <v>97</v>
-      </c>
+      <c r="N12" s="7"/>
     </row>
     <row r="13" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="C13" s="12">
         <v>43784</v>
@@ -1567,90 +1751,92 @@
       <c r="L13" s="11">
         <v>1</v>
       </c>
-      <c r="M13" s="24" t="s">
+      <c r="M13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="N13" s="19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="12">
+        <v>43784</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14" s="11">
+        <v>3</v>
+      </c>
+      <c r="L14" s="11">
+        <v>1</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="N14" s="19" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+    <row r="15" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B15" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C15" s="10">
         <v>43787</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K14" s="7">
-        <v>2</v>
-      </c>
-      <c r="L14" s="7">
-        <v>1</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N14" s="7"/>
-    </row>
-    <row r="15" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" s="12">
-        <v>43798</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="L15" s="11">
+      <c r="D15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="7">
+        <v>2</v>
+      </c>
+      <c r="L15" s="7">
         <v>1</v>
       </c>
       <c r="M15" s="3" t="s">
@@ -1660,165 +1846,169 @@
     </row>
     <row r="16" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C16" s="12">
+        <v>43789</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="11">
+        <v>3</v>
+      </c>
+      <c r="L16" s="11">
+        <v>0</v>
+      </c>
+      <c r="M16" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="N16" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C17" s="12">
+        <v>43789</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="11">
+        <v>2</v>
+      </c>
+      <c r="L17" s="11">
+        <v>0</v>
+      </c>
+      <c r="M17" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="N17" s="19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="12">
+        <v>43798</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="L18" s="11">
+        <v>1</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="19" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B19" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C19" s="12">
         <v>43799</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D19" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="25">
+      <c r="E19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="25">
         <v>4</v>
       </c>
-      <c r="L16" s="25">
-        <v>1</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N16" s="7"/>
-    </row>
-    <row r="17" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="10">
-        <v>43800</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="10">
-        <v>43800</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K18" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="L18" s="25">
-        <v>0</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N18" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="10">
-        <v>43800</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K19" s="7">
-        <v>3</v>
-      </c>
-      <c r="L19" s="7">
+      <c r="L19" s="25">
         <v>1</v>
       </c>
       <c r="M19" s="3" t="s">
@@ -1828,10 +2018,10 @@
     </row>
     <row r="20" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="C20" s="10">
         <v>43800</v>
@@ -1843,191 +2033,193 @@
         <v>20</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K20" s="7">
-        <v>3</v>
-      </c>
-      <c r="L20" s="7">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="M20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N20" s="7"/>
+      <c r="N20" s="7" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="21" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="C21" s="10">
         <v>43800</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>20</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="7"/>
       <c r="G21" s="7" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>20</v>
       </c>
       <c r="I21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" s="25">
+        <v>0</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="10">
+        <v>43800</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="7">
+        <v>3</v>
+      </c>
+      <c r="L22" s="7">
+        <v>1</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N22" s="7"/>
+    </row>
+    <row r="23" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="10">
+        <v>43800</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J21" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K21" s="7">
+      <c r="J23" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" s="7">
         <v>3</v>
       </c>
-      <c r="L21" s="7">
+      <c r="L23" s="7">
         <v>1</v>
       </c>
-      <c r="M21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N21" s="7"/>
-    </row>
-    <row r="22" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="12">
+      <c r="M23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N23" s="7"/>
+    </row>
+    <row r="24" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="10">
         <v>43800</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I22" s="11" t="s">
+      <c r="D24" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K22" s="11">
+      <c r="J24" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="7">
         <v>3</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L24" s="7">
         <v>1</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N22" s="7"/>
-    </row>
-    <row r="23" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" s="12">
-        <v>43800</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K23" s="25">
-        <v>3</v>
-      </c>
-      <c r="L23" s="25">
-        <v>1</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N23" s="7"/>
-    </row>
-    <row r="24" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" s="12">
-        <v>43800</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25">
-        <v>0</v>
       </c>
       <c r="M24" s="3" t="s">
         <v>23</v>
@@ -2037,10 +2229,10 @@
     </row>
     <row r="25" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="C25" s="12">
         <v>43800</v>
@@ -2061,18 +2253,18 @@
         <v>20</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="J25" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="11" t="s">
         <v>23</v>
       </c>
       <c r="K25" s="11">
         <v>3</v>
       </c>
-      <c r="L25" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M25" s="24" t="s">
+      <c r="L25" s="11">
+        <v>1</v>
+      </c>
+      <c r="M25" s="3" t="s">
         <v>23</v>
       </c>
       <c r="N25" s="7"/>
@@ -2080,16 +2272,16 @@
     </row>
     <row r="26" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="C26" s="12">
         <v>43800</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>2</v>
+      <c r="D26" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>20</v>
@@ -2109,13 +2301,13 @@
       <c r="J26" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K26" s="11">
+      <c r="K26" s="25">
         <v>3</v>
       </c>
-      <c r="L26" s="11">
+      <c r="L26" s="25">
         <v>1</v>
       </c>
-      <c r="M26" s="24" t="s">
+      <c r="M26" s="3" t="s">
         <v>23</v>
       </c>
       <c r="N26" s="7"/>
@@ -2123,16 +2315,16 @@
     </row>
     <row r="27" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="C27" s="12">
         <v>43800</v>
       </c>
-      <c r="D27" s="13" t="s">
-        <v>2</v>
+      <c r="D27" s="16" t="s">
+        <v>102</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>20</v>
@@ -2152,13 +2344,11 @@
       <c r="J27" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K27" s="11">
-        <v>3</v>
-      </c>
-      <c r="L27" s="11">
-        <v>1</v>
-      </c>
-      <c r="M27" s="24" t="s">
+      <c r="K27" s="25"/>
+      <c r="L27" s="25">
+        <v>0</v>
+      </c>
+      <c r="M27" s="3" t="s">
         <v>23</v>
       </c>
       <c r="N27" s="7"/>
@@ -2166,10 +2356,10 @@
     </row>
     <row r="28" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="C28" s="12">
         <v>43800</v>
@@ -2190,16 +2380,16 @@
         <v>20</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="J28" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J28" s="15" t="s">
         <v>23</v>
       </c>
       <c r="K28" s="11">
         <v>3</v>
       </c>
-      <c r="L28" s="11">
-        <v>1</v>
+      <c r="L28" s="11" t="s">
+        <v>27</v>
       </c>
       <c r="M28" s="24" t="s">
         <v>23</v>
@@ -2209,22 +2399,22 @@
     </row>
     <row r="29" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C29" s="12">
         <v>43800</v>
       </c>
-      <c r="D29" s="16" t="s">
-        <v>132</v>
+      <c r="D29" s="13" t="s">
+        <v>2</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>20</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="G29" s="11" t="s">
         <v>20</v>
@@ -2233,16 +2423,16 @@
         <v>20</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J29" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="K29" s="25">
+      <c r="K29" s="11">
         <v>3</v>
       </c>
-      <c r="L29" s="25">
-        <v>0</v>
+      <c r="L29" s="11">
+        <v>1</v>
       </c>
       <c r="M29" s="24" t="s">
         <v>23</v>
@@ -2252,15 +2442,15 @@
     </row>
     <row r="30" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="C30" s="12">
-        <v>43801</v>
-      </c>
-      <c r="D30" s="18" t="s">
+        <v>43800</v>
+      </c>
+      <c r="D30" s="13" t="s">
         <v>2</v>
       </c>
       <c r="E30" s="14" t="s">
@@ -2284,10 +2474,10 @@
       <c r="K30" s="11">
         <v>3</v>
       </c>
-      <c r="L30" s="15">
+      <c r="L30" s="11">
         <v>1</v>
       </c>
-      <c r="M30" s="3" t="s">
+      <c r="M30" s="24" t="s">
         <v>23</v>
       </c>
       <c r="N30" s="7"/>
@@ -2295,13 +2485,13 @@
     </row>
     <row r="31" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="C31" s="12">
-        <v>43801</v>
+        <v>43800</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>2</v>
@@ -2319,7 +2509,7 @@
         <v>20</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J31" s="11" t="s">
         <v>23</v>
@@ -2333,193 +2523,193 @@
       <c r="M31" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="N31" s="19" t="s">
-        <v>119</v>
-      </c>
+      <c r="N31" s="7"/>
       <c r="O31" s="2"/>
     </row>
     <row r="32" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="12">
+        <v>43800</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I32" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K32" s="25">
+        <v>3</v>
+      </c>
+      <c r="L32" s="25">
         <v>0</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="10">
-        <v>43805</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J32" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="K32" s="7">
-        <v>3</v>
-      </c>
-      <c r="L32" s="7">
-        <v>1</v>
-      </c>
-      <c r="M32" s="3" t="s">
+      <c r="M32" s="24" t="s">
         <v>23</v>
       </c>
       <c r="N32" s="7"/>
       <c r="O32" s="2"/>
     </row>
     <row r="33" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="C33" s="12">
-        <v>43806</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E33" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I33" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="J33" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K33" s="11">
+      <c r="A33" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="10">
+        <v>43800</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K33" s="7">
+        <v>2</v>
+      </c>
+      <c r="L33" s="7">
+        <v>0</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" s="12">
+        <v>43801</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K34" s="11">
         <v>3</v>
       </c>
-      <c r="L33" s="11">
+      <c r="L34" s="15">
         <v>1</v>
       </c>
-      <c r="M33" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="N33" s="7"/>
-      <c r="O33" s="2"/>
-    </row>
-    <row r="34" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C34" s="10">
-        <v>43814</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I34" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K34" s="7">
+      <c r="M34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N34" s="7"/>
+      <c r="O34" s="2"/>
+    </row>
+    <row r="35" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="12">
+        <v>43801</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K35" s="11">
         <v>3</v>
       </c>
-      <c r="L34" s="7">
+      <c r="L35" s="11">
         <v>1</v>
       </c>
-      <c r="M34" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N34" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="O34" s="2"/>
-    </row>
-    <row r="35" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="10">
-        <v>43814</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K35" s="7">
-        <v>3</v>
-      </c>
-      <c r="L35" s="7">
-        <v>1</v>
-      </c>
-      <c r="M35" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N35" s="7"/>
+      <c r="M35" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N35" s="19" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="36" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="C36" s="10">
-        <v>43815</v>
+        <v>43805</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>2</v>
@@ -2528,10 +2718,10 @@
         <v>20</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H36" s="7" t="s">
         <v>20</v>
@@ -2540,7 +2730,7 @@
         <v>23</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K36" s="7">
         <v>3</v>
@@ -2554,58 +2744,58 @@
       <c r="N36" s="7"/>
     </row>
     <row r="37" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" s="12">
+        <v>43806</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="11">
         <v>3</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="10">
-        <v>43834</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K37" s="7">
-        <v>3</v>
-      </c>
-      <c r="L37" s="7">
-        <v>0</v>
-      </c>
-      <c r="M37" s="7" t="s">
+      <c r="L37" s="11">
+        <v>1</v>
+      </c>
+      <c r="M37" s="11" t="s">
         <v>23</v>
       </c>
       <c r="N37" s="7"/>
     </row>
     <row r="38" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="C38" s="12">
-        <v>43836</v>
-      </c>
-      <c r="D38" s="13" t="s">
+        <v>43806</v>
+      </c>
+      <c r="D38" s="18" t="s">
         <v>2</v>
       </c>
       <c r="E38" s="14" t="s">
@@ -2635,59 +2825,63 @@
       <c r="M38" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="N38" s="7"/>
+      <c r="N38" s="19" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="39" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" s="10">
-        <v>43847</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I39" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J39" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K39" s="7">
+      <c r="A39" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C39" s="12">
+        <v>43812</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K39" s="11">
         <v>3</v>
       </c>
-      <c r="L39" s="7">
-        <v>1</v>
-      </c>
-      <c r="M39" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N39" s="7"/>
+      <c r="L39" s="11">
+        <v>0</v>
+      </c>
+      <c r="M39" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N39" s="19" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="40" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C40" s="10">
-        <v>44043</v>
+        <v>43814</v>
       </c>
       <c r="D40" s="8" t="s">
         <v>2</v>
@@ -2719,35 +2913,37 @@
       <c r="M40" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N40" s="7"/>
+      <c r="N40" s="7" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="41" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="C41" s="10">
-        <v>44044</v>
+        <v>43814</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>2</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G41" s="7" t="s">
         <v>20</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J41" s="7" t="s">
         <v>23</v>
@@ -2755,8 +2951,8 @@
       <c r="K41" s="7">
         <v>3</v>
       </c>
-      <c r="L41" s="7" t="s">
-        <v>27</v>
+      <c r="L41" s="7">
+        <v>1</v>
       </c>
       <c r="M41" s="7" t="s">
         <v>23</v>
@@ -2765,22 +2961,22 @@
     </row>
     <row r="42" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C42" s="10">
-        <v>44166</v>
+        <v>43815</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>84</v>
+        <v>2</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G42" s="7" t="s">
         <v>20</v>
@@ -2789,117 +2985,662 @@
         <v>20</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J42" s="7" t="s">
         <v>23</v>
       </c>
       <c r="K42" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L42" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M42" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N42" s="7" t="s">
-        <v>85</v>
-      </c>
+      <c r="N42" s="7"/>
     </row>
     <row r="43" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B43" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="10">
+        <v>43834</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K43" s="7">
+        <v>3</v>
+      </c>
+      <c r="L43" s="7">
+        <v>0</v>
+      </c>
+      <c r="M43" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N43" s="7"/>
+    </row>
+    <row r="44" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="12">
+        <v>43836</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I44" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J44" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K44" s="11">
+        <v>3</v>
+      </c>
+      <c r="L44" s="11">
+        <v>1</v>
+      </c>
+      <c r="M44" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N44" s="7"/>
+    </row>
+    <row r="45" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" s="10">
+        <v>43847</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J45" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K45" s="7">
+        <v>3</v>
+      </c>
+      <c r="L45" s="7">
+        <v>1</v>
+      </c>
+      <c r="M45" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N45" s="7"/>
+    </row>
+    <row r="46" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="10">
+        <v>44043</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J46" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K46" s="7">
+        <v>3</v>
+      </c>
+      <c r="L46" s="7">
+        <v>1</v>
+      </c>
+      <c r="M46" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N46" s="7"/>
+    </row>
+    <row r="47" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="10">
+        <v>44044</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K47" s="7">
+        <v>3</v>
+      </c>
+      <c r="L47" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M47" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N47" s="7"/>
+    </row>
+    <row r="48" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C48" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K43" s="7" t="s">
+      <c r="D48" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J48" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K48" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L43" s="7">
+      <c r="L48" s="7">
         <v>1</v>
       </c>
-      <c r="M43" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N43" s="7"/>
-    </row>
-    <row r="44" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
+      <c r="M48" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N48" s="7"/>
+    </row>
+    <row r="49" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B49" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C44" s="7"/>
-      <c r="D44" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I44" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J44" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K44" s="7">
+      <c r="C49" s="7"/>
+      <c r="D49" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J49" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K49" s="7">
         <v>3</v>
       </c>
-      <c r="L44" s="7">
+      <c r="L49" s="7">
         <v>1</v>
       </c>
-      <c r="M44" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N44" s="7" t="s">
+      <c r="M49" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N49" s="7" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N44">
-    <sortCondition ref="C2:C44"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N49">
+    <sortCondition ref="C2:C49"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="D16" r:id="rId1" display="https://recruit.ucdavis.edu/JPF02950" xr:uid="{83E02472-223D-514A-82F7-94F8C5C76C6F}"/>
-    <hyperlink ref="D24" r:id="rId2" xr:uid="{A94B9440-F8F2-1D40-B6F8-BDDE35FB8D62}"/>
-    <hyperlink ref="D29" r:id="rId3" xr:uid="{4B367342-2FC3-E140-A9EC-CB0227AE528A}"/>
+    <hyperlink ref="D19" r:id="rId1" display="https://recruit.ucdavis.edu/JPF02950" xr:uid="{83E02472-223D-514A-82F7-94F8C5C76C6F}"/>
+    <hyperlink ref="D27" r:id="rId2" xr:uid="{A94B9440-F8F2-1D40-B6F8-BDDE35FB8D62}"/>
+    <hyperlink ref="D32" r:id="rId3" xr:uid="{4B367342-2FC3-E140-A9EC-CB0227AE528A}"/>
+    <hyperlink ref="D16" r:id="rId4" display="https://www.vacancies.ed.ac.uk/pls/corehrrecruit/erq_jobspec_version_4.jobspec?p_id=050154" xr:uid="{200AE473-7A60-B148-BA2A-18A77C170360}"/>
+    <hyperlink ref="D17" r:id="rId5" display="https://www.recruit.ox.ac.uk/pls/hrisliverecruit/erq_jobspec_version_4.jobspec?p_id=143481" xr:uid="{07A2CD43-8F6C-854C-9BA5-EE4023673833}"/>
+    <hyperlink ref="D39" r:id="rId6" xr:uid="{155296AC-9F8B-B042-9832-B901625AED63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7E1F877-7631-084F-B95D-E28DC512FF41}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="33"/>
+    <col min="4" max="8" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="30">
+        <v>43770</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="31">
+        <v>43770</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G3" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" s="32">
+        <v>43789</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5" s="32">
+        <v>43789</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="32">
+        <v>43799</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="G6" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="H6" s="40" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="31">
+        <v>43800</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="32">
+        <v>43800</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="H8" s="40" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="32">
+        <v>43800</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C10" s="32">
+        <v>43800</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="31">
+        <v>43800</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="32">
+        <v>43812</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G12" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Many Jobs Applied For
</commit_message>
<xml_diff>
--- a/Postdocs19.xlsx
+++ b/Postdocs19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DJBruce/Application-Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EDAF396-8F41-7D4C-AAED-8BE4945ECE75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14349B1-49D4-3243-916F-280B9C1575B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" xr2:uid="{FC4BAEE4-913F-A74A-BB8A-E591CDEA97CC}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="173">
   <si>
     <t xml:space="preserve">Arizona State University </t>
   </si>
@@ -124,15 +124,6 @@
     <t>1118-POSTDOC</t>
   </si>
   <si>
-    <t>FSU-SJPS</t>
-  </si>
-  <si>
-    <t>3?</t>
-  </si>
-  <si>
-    <t>Florida State University?</t>
-  </si>
-  <si>
     <t>Georgia Institute of Technology</t>
   </si>
   <si>
@@ -529,9 +520,6 @@
     <t>Requested 10/21/19</t>
   </si>
   <si>
-    <t>Re-Request 10/21/19</t>
-  </si>
-  <si>
     <t>Request Need</t>
   </si>
   <si>
@@ -554,6 +542,15 @@
   </si>
   <si>
     <t>Yes, non-expert</t>
+  </si>
+  <si>
+    <t>Uploaded 10/26/19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tufts University </t>
+  </si>
+  <si>
+    <t>Tufts-NWAPALGEBRA</t>
   </si>
 </sst>
 </file>
@@ -768,7 +765,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -914,6 +911,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1238,8 +1241,8 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9:N9"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1253,16 +1256,16 @@
   <sheetData>
     <row r="1" spans="1:14" ht="70" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>83</v>
-      </c>
       <c r="C1" s="17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>18</v>
@@ -1292,15 +1295,15 @@
         <v>17</v>
       </c>
       <c r="N1" s="17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="70" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C2" s="45">
         <v>43770</v>
@@ -1336,87 +1339,87 @@
         <v>23</v>
       </c>
       <c r="N2" s="44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="7">
+      <c r="A3" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="41">
         <v>43770</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="D3" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="4" t="s">
+      <c r="J3" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="40">
         <v>1</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>77</v>
+      <c r="M3" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="40" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" s="7">
         <v>43770</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>23</v>
@@ -1424,181 +1427,181 @@
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="7">
+      <c r="A5" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="41">
         <v>43770</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="4">
-        <v>3</v>
-      </c>
-      <c r="L5" s="4" t="s">
+      <c r="D5" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="40">
+        <v>3</v>
+      </c>
+      <c r="L5" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N5" s="4"/>
+      <c r="M5" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="40"/>
     </row>
     <row r="6" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="9">
+      <c r="A6" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="48">
         <v>43770</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="8">
-        <v>3</v>
-      </c>
-      <c r="L6" s="8" t="s">
+      <c r="D6" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="40">
+        <v>3</v>
+      </c>
+      <c r="L6" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N6" s="16" t="s">
-        <v>91</v>
+      <c r="M6" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="49" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" s="9">
+      <c r="A7" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="48">
         <v>43770</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="8">
-        <v>3</v>
-      </c>
-      <c r="L7" s="12">
+      <c r="D7" s="50" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="40">
+        <v>3</v>
+      </c>
+      <c r="L7" s="51">
         <v>1</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N7" s="4"/>
+      <c r="M7" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="N7" s="40"/>
     </row>
     <row r="8" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C8" s="9">
+      <c r="A8" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="48">
         <v>43770</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="8">
-        <v>3</v>
-      </c>
-      <c r="L8" s="8" t="s">
+      <c r="D8" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="40">
+        <v>3</v>
+      </c>
+      <c r="L8" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="N8" s="4"/>
+      <c r="M8" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="N8" s="40"/>
     </row>
     <row r="9" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="40" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C9" s="48">
         <v>43770</v>
@@ -1634,39 +1637,39 @@
         <v>23</v>
       </c>
       <c r="N9" s="49" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C10" s="9">
         <v>43770</v>
       </c>
       <c r="D10" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>173</v>
-      </c>
       <c r="H10" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>23</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="K10" s="8">
         <v>3</v>
@@ -1678,141 +1681,143 @@
         <v>23</v>
       </c>
       <c r="N10" s="39" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="41">
         <v>43773</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" s="4">
-        <v>3</v>
-      </c>
-      <c r="L11" s="4">
+      <c r="D11" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="40">
+        <v>3</v>
+      </c>
+      <c r="L11" s="40">
         <v>1</v>
       </c>
-      <c r="M11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N11" s="4"/>
+      <c r="M11" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11" s="40"/>
     </row>
     <row r="12" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="7">
+      <c r="A12" s="40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="41">
         <v>43784</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N12" s="4"/>
+      <c r="D12" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="40">
+        <v>3</v>
+      </c>
+      <c r="L12" s="40">
+        <v>1</v>
+      </c>
+      <c r="M12" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" s="40"/>
     </row>
     <row r="13" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="7">
+      <c r="A13" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="48">
         <v>43784</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13" s="4">
-        <v>3</v>
-      </c>
-      <c r="L13" s="4">
+      <c r="D13" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="40">
+        <v>3</v>
+      </c>
+      <c r="L13" s="40">
         <v>1</v>
       </c>
-      <c r="M13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N13" s="4"/>
+      <c r="M13" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="N13" s="49" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="14" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="C14" s="9">
         <v>43784</v>
@@ -1844,114 +1849,114 @@
       <c r="L14" s="8">
         <v>1</v>
       </c>
-      <c r="M14" s="3" t="s">
+      <c r="M14" s="21" t="s">
         <v>23</v>
       </c>
       <c r="N14" s="16" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C15" s="9">
-        <v>43784</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="8">
-        <v>3</v>
-      </c>
-      <c r="L15" s="8">
+      <c r="A15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="7">
+        <v>43787</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="4">
+        <v>2</v>
+      </c>
+      <c r="L15" s="4">
         <v>1</v>
       </c>
-      <c r="M15" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="N15" s="16" t="s">
-        <v>112</v>
-      </c>
+      <c r="M15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="7">
-        <v>43787</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K16" s="4">
-        <v>2</v>
-      </c>
-      <c r="L16" s="4">
-        <v>1</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N16" s="4"/>
+      <c r="A16" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C16" s="9">
+        <v>43789</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K16" s="8">
+        <v>3</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="N16" s="16" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="17" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B17" s="8" t="s">
         <v>134</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>135</v>
       </c>
       <c r="C17" s="9">
         <v>43789</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>23</v>
@@ -1969,7 +1974,7 @@
         <v>23</v>
       </c>
       <c r="K17" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L17" s="8">
         <v>0</v>
@@ -1978,24 +1983,24 @@
         <v>23</v>
       </c>
       <c r="N17" s="16" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>138</v>
+        <v>89</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="C18" s="9">
-        <v>43789</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>139</v>
+        <v>43798</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>2</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>23</v>
@@ -2007,42 +2012,40 @@
         <v>20</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="8">
-        <v>2</v>
+      <c r="K18" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="L18" s="8">
-        <v>0</v>
-      </c>
-      <c r="M18" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="N18" s="16" t="s">
-        <v>140</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C19" s="9">
-        <v>43798</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>2</v>
+        <v>43799</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>102</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>20</v>
@@ -2056,10 +2059,10 @@
       <c r="J19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="L19" s="8">
+      <c r="K19" s="22">
+        <v>4</v>
+      </c>
+      <c r="L19" s="22">
         <v>1</v>
       </c>
       <c r="M19" s="3" t="s">
@@ -2068,137 +2071,137 @@
       <c r="N19" s="4"/>
     </row>
     <row r="20" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="9">
-        <v>43799</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K20" s="22">
-        <v>4</v>
-      </c>
-      <c r="L20" s="22">
+      <c r="A20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="7">
+        <v>43800</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="41">
+        <v>43800</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="43"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="J21" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="L21" s="40">
+        <v>0</v>
+      </c>
+      <c r="M21" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="N21" s="40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="7">
+        <v>43800</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" s="4">
+        <v>3</v>
+      </c>
+      <c r="L22" s="4">
         <v>1</v>
       </c>
-      <c r="M20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N20" s="4"/>
-    </row>
-    <row r="21" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="7">
-        <v>43800</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="41">
-        <v>43800</v>
-      </c>
-      <c r="D22" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="43"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="H22" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="I22" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="J22" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="K22" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="L22" s="40">
-        <v>0</v>
-      </c>
-      <c r="M22" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="N22" s="40" t="s">
-        <v>52</v>
-      </c>
+      <c r="M22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N22" s="4"/>
     </row>
     <row r="23" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C23" s="7">
         <v>43800</v>
@@ -2210,16 +2213,16 @@
         <v>20</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J23" s="4" t="s">
         <v>23</v>
@@ -2234,6 +2237,7 @@
         <v>23</v>
       </c>
       <c r="N23" s="4"/>
+      <c r="O23" s="2"/>
     </row>
     <row r="24" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
@@ -2252,10 +2256,10 @@
         <v>20</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>20</v>
@@ -2279,40 +2283,40 @@
       <c r="O24" s="2"/>
     </row>
     <row r="25" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C25" s="7">
+      <c r="A25" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="9">
         <v>43800</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I25" s="4" t="s">
+      <c r="D25" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="J25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K25" s="4">
-        <v>3</v>
-      </c>
-      <c r="L25" s="4">
+      <c r="J25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="8">
+        <v>3</v>
+      </c>
+      <c r="L25" s="8">
         <v>1</v>
       </c>
       <c r="M25" s="3" t="s">
@@ -2323,16 +2327,16 @@
     </row>
     <row r="26" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C26" s="9">
         <v>43800</v>
       </c>
-      <c r="D26" s="10" t="s">
-        <v>2</v>
+      <c r="D26" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="E26" s="11" t="s">
         <v>20</v>
@@ -2347,15 +2351,15 @@
         <v>20</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J26" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K26" s="8">
-        <v>3</v>
-      </c>
-      <c r="L26" s="8">
+      <c r="K26" s="22">
+        <v>3</v>
+      </c>
+      <c r="L26" s="22">
         <v>1</v>
       </c>
       <c r="M26" s="3" t="s">
@@ -2366,16 +2370,16 @@
     </row>
     <row r="27" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>99</v>
       </c>
       <c r="C27" s="9">
         <v>43800</v>
       </c>
-      <c r="D27" s="20" t="s">
-        <v>100</v>
+      <c r="D27" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>20</v>
@@ -2395,11 +2399,9 @@
       <c r="J27" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K27" s="22">
-        <v>3</v>
-      </c>
+      <c r="K27" s="22"/>
       <c r="L27" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M27" s="3" t="s">
         <v>23</v>
@@ -2409,16 +2411,16 @@
     </row>
     <row r="28" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="C28" s="9">
         <v>43800</v>
       </c>
-      <c r="D28" s="13" t="s">
-        <v>102</v>
+      <c r="D28" s="10" t="s">
+        <v>2</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>20</v>
@@ -2433,16 +2435,18 @@
         <v>20</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22">
-        <v>0</v>
-      </c>
-      <c r="M28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" s="8">
+        <v>3</v>
+      </c>
+      <c r="L28" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="M28" s="21" t="s">
         <v>23</v>
       </c>
       <c r="N28" s="4"/>
@@ -2450,10 +2454,10 @@
     </row>
     <row r="29" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C29" s="9">
         <v>43800</v>
@@ -2474,16 +2478,16 @@
         <v>20</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="J29" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J29" s="8" t="s">
         <v>23</v>
       </c>
       <c r="K29" s="8">
         <v>3</v>
       </c>
-      <c r="L29" s="8" t="s">
-        <v>27</v>
+      <c r="L29" s="8">
+        <v>1</v>
       </c>
       <c r="M29" s="21" t="s">
         <v>23</v>
@@ -2493,10 +2497,10 @@
     </row>
     <row r="30" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C30" s="9">
         <v>43800</v>
@@ -2536,10 +2540,10 @@
     </row>
     <row r="31" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C31" s="9">
         <v>43800</v>
@@ -2560,7 +2564,7 @@
         <v>20</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J31" s="8" t="s">
         <v>23</v>
@@ -2579,22 +2583,22 @@
     </row>
     <row r="32" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>129</v>
       </c>
       <c r="C32" s="9">
         <v>43800</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>2</v>
+      <c r="D32" s="13" t="s">
+        <v>129</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>20</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>20</v>
@@ -2608,11 +2612,11 @@
       <c r="J32" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K32" s="8">
-        <v>3</v>
-      </c>
-      <c r="L32" s="8">
-        <v>1</v>
+      <c r="K32" s="22">
+        <v>3</v>
+      </c>
+      <c r="L32" s="22">
+        <v>0</v>
       </c>
       <c r="M32" s="21" t="s">
         <v>23</v>
@@ -2621,104 +2625,103 @@
       <c r="O32" s="2"/>
     </row>
     <row r="33" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="C33" s="9">
+      <c r="A33" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="7">
         <v>43800</v>
       </c>
-      <c r="D33" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J33" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K33" s="22">
-        <v>3</v>
-      </c>
-      <c r="L33" s="22">
+      <c r="D33" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K33" s="4">
+        <v>2</v>
+      </c>
+      <c r="L33" s="4">
         <v>0</v>
       </c>
-      <c r="M33" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="N33" s="4"/>
+      <c r="M33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="O33" s="2"/>
     </row>
     <row r="34" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="7">
-        <v>43800</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K34" s="4">
-        <v>2</v>
-      </c>
-      <c r="L34" s="4">
-        <v>0</v>
-      </c>
-      <c r="M34" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N34" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="O34" s="2"/>
+      <c r="A34" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34" s="9">
+        <v>43801</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K34" s="8">
+        <v>3</v>
+      </c>
+      <c r="L34" s="12">
+        <v>1</v>
+      </c>
+      <c r="M34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N34" s="4"/>
     </row>
     <row r="35" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C35" s="9">
         <v>43801</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E35" s="11" t="s">
@@ -2742,115 +2745,115 @@
       <c r="K35" s="8">
         <v>3</v>
       </c>
-      <c r="L35" s="12">
+      <c r="L35" s="8">
         <v>1</v>
       </c>
-      <c r="M35" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N35" s="4"/>
+      <c r="M35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N35" s="16" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="36" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="C36" s="9">
-        <v>43801</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E36" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K36" s="8">
-        <v>3</v>
-      </c>
-      <c r="L36" s="8">
+      <c r="A36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M36" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N36" s="16" t="s">
-        <v>119</v>
-      </c>
+      <c r="C36" s="7">
+        <v>43805</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" s="4">
+        <v>3</v>
+      </c>
+      <c r="L36" s="4">
+        <v>1</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N36" s="4"/>
     </row>
     <row r="37" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="4" t="s">
+      <c r="A37" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" s="9">
+        <v>43806</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="8">
+        <v>3</v>
+      </c>
+      <c r="L37" s="8">
         <v>1</v>
       </c>
-      <c r="C37" s="7">
-        <v>43805</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K37" s="4">
-        <v>3</v>
-      </c>
-      <c r="L37" s="4">
-        <v>1</v>
-      </c>
-      <c r="M37" s="4" t="s">
+      <c r="M37" s="8" t="s">
         <v>23</v>
       </c>
       <c r="N37" s="4"/>
     </row>
     <row r="38" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="C38" s="9">
         <v>43806</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="15" t="s">
         <v>2</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>20</v>
@@ -2876,35 +2879,37 @@
       <c r="M38" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="N38" s="4"/>
+      <c r="N38" s="16" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="39" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C39" s="9">
-        <v>43806</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>2</v>
+        <v>43812</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>143</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>20</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>20</v>
+        <v>145</v>
       </c>
       <c r="J39" s="8" t="s">
         <v>23</v>
@@ -2913,65 +2918,65 @@
         <v>3</v>
       </c>
       <c r="L39" s="8">
+        <v>0</v>
+      </c>
+      <c r="M39" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="N39" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="7">
+        <v>43814</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K40" s="4">
+        <v>3</v>
+      </c>
+      <c r="L40" s="4">
         <v>1</v>
       </c>
-      <c r="M39" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N39" s="16" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="C40" s="9">
-        <v>43812</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G40" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H40" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="I40" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K40" s="8">
-        <v>3</v>
-      </c>
-      <c r="L40" s="8">
-        <v>0</v>
-      </c>
-      <c r="M40" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="N40" s="16" t="s">
-        <v>149</v>
+      <c r="M40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="C41" s="7">
         <v>43814</v>
@@ -2980,7 +2985,7 @@
         <v>2</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="F41" s="4" t="s">
         <v>20</v>
@@ -2989,10 +2994,10 @@
         <v>20</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J41" s="4" t="s">
         <v>23</v>
@@ -3006,58 +3011,56 @@
       <c r="M41" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N41" s="4" t="s">
-        <v>78</v>
-      </c>
+      <c r="N41" s="4"/>
     </row>
     <row r="42" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="7">
+      <c r="A42" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C42" s="9">
         <v>43814</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K42" s="4">
-        <v>3</v>
-      </c>
-      <c r="L42" s="4">
-        <v>1</v>
-      </c>
-      <c r="M42" s="4" t="s">
+      <c r="D42" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K42" s="8">
+        <v>3</v>
+      </c>
+      <c r="L42" s="8">
+        <v>0</v>
+      </c>
+      <c r="M42" s="8" t="s">
         <v>23</v>
       </c>
       <c r="N42" s="4"/>
     </row>
     <row r="43" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C43" s="7">
         <v>43815</v>
@@ -3095,53 +3098,53 @@
       <c r="N43" s="4"/>
     </row>
     <row r="44" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B44" s="4" t="s">
+      <c r="A44" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="41">
         <v>43834</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I44" s="4" t="s">
+      <c r="D44" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="G44" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="H44" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="I44" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="J44" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K44" s="4">
-        <v>3</v>
-      </c>
-      <c r="L44" s="4">
+      <c r="J44" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="K44" s="40">
+        <v>3</v>
+      </c>
+      <c r="L44" s="40">
         <v>0</v>
       </c>
-      <c r="M44" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N44" s="4"/>
+      <c r="M44" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="N44" s="40"/>
     </row>
     <row r="45" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C45" s="9">
         <v>43836</v>
@@ -3180,10 +3183,10 @@
     </row>
     <row r="46" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C46" s="7">
         <v>43847</v>
@@ -3192,7 +3195,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F46" s="4" t="s">
         <v>20</v>
@@ -3222,10 +3225,10 @@
     </row>
     <row r="47" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C47" s="7">
         <v>44043</v>
@@ -3264,10 +3267,10 @@
     </row>
     <row r="48" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C48" s="7">
         <v>44044</v>
@@ -3285,7 +3288,7 @@
         <v>20</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I48" s="4" t="s">
         <v>20</v>
@@ -3385,7 +3388,7 @@
         <v>20</v>
       </c>
       <c r="N50" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -3393,12 +3396,12 @@
     <sortCondition ref="C2:C50"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="D20" r:id="rId1" display="https://recruit.ucdavis.edu/JPF02950" xr:uid="{83E02472-223D-514A-82F7-94F8C5C76C6F}"/>
-    <hyperlink ref="D28" r:id="rId2" xr:uid="{A94B9440-F8F2-1D40-B6F8-BDDE35FB8D62}"/>
-    <hyperlink ref="D33" r:id="rId3" xr:uid="{4B367342-2FC3-E140-A9EC-CB0227AE528A}"/>
-    <hyperlink ref="D17" r:id="rId4" display="https://www.vacancies.ed.ac.uk/pls/corehrrecruit/erq_jobspec_version_4.jobspec?p_id=050154" xr:uid="{200AE473-7A60-B148-BA2A-18A77C170360}"/>
-    <hyperlink ref="D18" r:id="rId5" display="https://www.recruit.ox.ac.uk/pls/hrisliverecruit/erq_jobspec_version_4.jobspec?p_id=143481" xr:uid="{07A2CD43-8F6C-854C-9BA5-EE4023673833}"/>
-    <hyperlink ref="D40" r:id="rId6" xr:uid="{155296AC-9F8B-B042-9832-B901625AED63}"/>
+    <hyperlink ref="D19" r:id="rId1" display="https://recruit.ucdavis.edu/JPF02950" xr:uid="{83E02472-223D-514A-82F7-94F8C5C76C6F}"/>
+    <hyperlink ref="D27" r:id="rId2" xr:uid="{A94B9440-F8F2-1D40-B6F8-BDDE35FB8D62}"/>
+    <hyperlink ref="D32" r:id="rId3" xr:uid="{4B367342-2FC3-E140-A9EC-CB0227AE528A}"/>
+    <hyperlink ref="D16" r:id="rId4" display="https://www.vacancies.ed.ac.uk/pls/corehrrecruit/erq_jobspec_version_4.jobspec?p_id=050154" xr:uid="{200AE473-7A60-B148-BA2A-18A77C170360}"/>
+    <hyperlink ref="D17" r:id="rId5" display="https://www.recruit.ox.ac.uk/pls/hrisliverecruit/erq_jobspec_version_4.jobspec?p_id=143481" xr:uid="{07A2CD43-8F6C-854C-9BA5-EE4023673833}"/>
+    <hyperlink ref="D39" r:id="rId6" xr:uid="{155296AC-9F8B-B042-9832-B901625AED63}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3410,7 +3413,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3423,33 +3426,33 @@
   <sheetData>
     <row r="1" spans="1:8" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="17" t="s">
-        <v>83</v>
-      </c>
       <c r="C1" s="18" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D1" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="H1" s="25" t="s">
         <v>153</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>2</v>
@@ -3458,279 +3461,279 @@
         <v>43770</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>164</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>165</v>
+        <v>161</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" s="28">
         <v>43770</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H3" s="32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C4" s="29">
         <v>43789</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F4" s="32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G4" s="36" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C5" s="29">
         <v>43789</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="G5" s="36" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H5" s="32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C6" s="29">
         <v>43799</v>
       </c>
       <c r="D6" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="E6" s="37" t="s">
-        <v>164</v>
-      </c>
       <c r="F6" s="32" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G6" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="H6" s="37" t="s">
-        <v>164</v>
+        <v>161</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="C7" s="28">
         <v>43800</v>
       </c>
       <c r="D7" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="E7" s="37" t="s">
-        <v>164</v>
-      </c>
       <c r="F7" s="32" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G7" s="37" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C8" s="29">
         <v>43800</v>
       </c>
       <c r="D8" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="E8" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="G8" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="H8" s="37" t="s">
-        <v>164</v>
+      <c r="H8" s="32" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>98</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>101</v>
       </c>
       <c r="C9" s="29">
         <v>43800</v>
       </c>
       <c r="D9" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="G9" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="E9" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="G9" s="37" t="s">
-        <v>164</v>
-      </c>
       <c r="H9" s="32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C10" s="29">
         <v>43800</v>
       </c>
       <c r="D10" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="G10" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="E10" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="G10" s="37" t="s">
-        <v>164</v>
-      </c>
       <c r="H10" s="32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C11" s="28">
         <v>43800</v>
       </c>
       <c r="D11" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="G11" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="E11" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="G11" s="37" t="s">
-        <v>164</v>
-      </c>
       <c r="H11" s="32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C12" s="29">
         <v>43812</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E12" s="32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G12" s="36" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="H12" s="32" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>